<commit_message>
Finish first 20 questions
</commit_message>
<xml_diff>
--- a/personality.xlsx
+++ b/personality.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="187">
   <si>
     <t>Question #</t>
   </si>
@@ -217,9 +217,6 @@
     <t>Love them!</t>
   </si>
   <si>
-    <t>I little. I'll have a sensible chuckle every now and then.</t>
-  </si>
-  <si>
     <t>Not really.</t>
   </si>
   <si>
@@ -481,6 +478,9 @@
     <t xml:space="preserve">Confident  </t>
   </si>
   <si>
+    <t>Confident, Confident, Confident</t>
+  </si>
+  <si>
     <t>Docile, Docile, Imaginative, Observant</t>
   </si>
   <si>
@@ -500,6 +500,93 @@
   </si>
   <si>
     <t>Imagination</t>
+  </si>
+  <si>
+    <t>Hardy, Hardy, Observant</t>
+  </si>
+  <si>
+    <t>Docile, Lonely</t>
+  </si>
+  <si>
+    <t>Confident, Jolly</t>
+  </si>
+  <si>
+    <t>Jolly, Jolly, Jolly</t>
+  </si>
+  <si>
+    <t>Lonely, Lonely</t>
+  </si>
+  <si>
+    <t>Lonely, Hardy</t>
+  </si>
+  <si>
+    <t>Jolly, Imaginative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confident, Confident, Hardy </t>
+  </si>
+  <si>
+    <t>Aggressive, Aggressive</t>
+  </si>
+  <si>
+    <t>Confident, Hasty, Aggressive</t>
+  </si>
+  <si>
+    <t>A little. I'll have a sensible chuckle every now and then.</t>
+  </si>
+  <si>
+    <t>Jolly, Imaginative, Lonely</t>
+  </si>
+  <si>
+    <t>Confident, Confident, Imaginative</t>
+  </si>
+  <si>
+    <t>Hasty, Hardy, Observant</t>
+  </si>
+  <si>
+    <t>Aggressive, Observant</t>
+  </si>
+  <si>
+    <t>Jolly, Jolly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hasty, Hasty </t>
+  </si>
+  <si>
+    <t>Observant, Observant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Docile, Observant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lonely, Lonely  </t>
+  </si>
+  <si>
+    <t>Hasty, Hasty, Jolly</t>
+  </si>
+  <si>
+    <t>Observant, Imaginative, Hardy</t>
+  </si>
+  <si>
+    <t>Docile, Jolly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observant </t>
+  </si>
+  <si>
+    <t>Imaginative, Imaginative, Hardy, Observant</t>
+  </si>
+  <si>
+    <t>Aggressive, Hasty</t>
+  </si>
+  <si>
+    <t>Hasty, Aggressive</t>
+  </si>
+  <si>
+    <t>Lonely, Lonely, Docile</t>
+  </si>
+  <si>
+    <t>Observant, Docile</t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1157,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1081,7 +1168,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1092,7 +1179,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1103,7 +1190,7 @@
         <v>7</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1114,7 +1201,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1223,10 +1310,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,7 +1325,7 @@
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1255,7 +1342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1263,16 +1350,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1280,16 +1367,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1297,19 +1381,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1317,19 +1398,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="H5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1337,19 +1415,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" t="s">
         <v>122</v>
-      </c>
-      <c r="D6" t="s">
-        <v>123</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1357,19 +1432,16 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="H7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1377,16 +1449,13 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E8" t="s">
         <v>18</v>
       </c>
-      <c r="H8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1394,16 +1463,13 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E9" t="s">
         <v>19</v>
       </c>
-      <c r="H9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1411,19 +1477,16 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
       </c>
-      <c r="H10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1431,19 +1494,16 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" t="s">
         <v>130</v>
-      </c>
-      <c r="D11" t="s">
-        <v>131</v>
       </c>
       <c r="E11" t="s">
         <v>21</v>
       </c>
-      <c r="H11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1451,13 +1511,13 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1465,16 +1525,16 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1482,16 +1542,16 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1499,16 +1559,16 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" t="s">
         <v>133</v>
-      </c>
-      <c r="D15" t="s">
-        <v>134</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1516,10 +1576,10 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E16" t="s">
         <v>27</v>
@@ -1533,10 +1593,10 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E17" t="s">
         <v>28</v>
@@ -1550,10 +1610,10 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
@@ -1567,10 +1627,10 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E19" t="s">
         <v>32</v>
@@ -1584,10 +1644,10 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
+        <v>139</v>
+      </c>
+      <c r="D20" t="s">
         <v>140</v>
-      </c>
-      <c r="D20" t="s">
-        <v>141</v>
       </c>
       <c r="E20" t="s">
         <v>31</v>
@@ -1601,10 +1661,10 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E21" t="s">
         <v>34</v>
@@ -1618,10 +1678,10 @@
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E22" t="s">
         <v>37</v>
@@ -1635,10 +1695,10 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E23" t="s">
         <v>36</v>
@@ -1652,7 +1712,7 @@
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E24" t="s">
         <v>35</v>
@@ -1666,10 +1726,10 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E25" t="s">
         <v>39</v>
@@ -1683,10 +1743,10 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E26" t="s">
         <v>40</v>
@@ -1700,10 +1760,10 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E27" t="s">
         <v>41</v>
@@ -1720,7 +1780,7 @@
         <v>152</v>
       </c>
       <c r="D28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E28" t="s">
         <v>43</v>
@@ -1751,7 +1811,7 @@
         <v>153</v>
       </c>
       <c r="D30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E30" t="s">
         <v>46</v>
@@ -1768,7 +1828,7 @@
         <v>154</v>
       </c>
       <c r="D31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E31" t="s">
         <v>47</v>
@@ -1802,7 +1862,7 @@
         <v>156</v>
       </c>
       <c r="D33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E33" t="s">
         <v>51</v>
@@ -1816,10 +1876,10 @@
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E34" t="s">
         <v>50</v>
@@ -1832,6 +1892,12 @@
       <c r="B35">
         <v>12</v>
       </c>
+      <c r="C35" t="s">
+        <v>146</v>
+      </c>
+      <c r="D35" t="s">
+        <v>90</v>
+      </c>
       <c r="E35" t="s">
         <v>53</v>
       </c>
@@ -1843,6 +1909,12 @@
       <c r="B36">
         <v>12</v>
       </c>
+      <c r="C36" t="s">
+        <v>158</v>
+      </c>
+      <c r="D36" t="s">
+        <v>92</v>
+      </c>
       <c r="E36" t="s">
         <v>54</v>
       </c>
@@ -1854,6 +1926,12 @@
       <c r="B37">
         <v>12</v>
       </c>
+      <c r="C37" t="s">
+        <v>159</v>
+      </c>
+      <c r="D37" t="s">
+        <v>160</v>
+      </c>
       <c r="E37" t="s">
         <v>55</v>
       </c>
@@ -1865,6 +1943,12 @@
       <c r="B38">
         <v>13</v>
       </c>
+      <c r="C38" t="s">
+        <v>161</v>
+      </c>
+      <c r="D38" t="s">
+        <v>90</v>
+      </c>
       <c r="E38" t="s">
         <v>24</v>
       </c>
@@ -1876,6 +1960,12 @@
       <c r="B39">
         <v>13</v>
       </c>
+      <c r="C39" t="s">
+        <v>163</v>
+      </c>
+      <c r="D39" t="s">
+        <v>164</v>
+      </c>
       <c r="E39" t="s">
         <v>25</v>
       </c>
@@ -1887,6 +1977,12 @@
       <c r="B40">
         <v>14</v>
       </c>
+      <c r="C40" t="s">
+        <v>165</v>
+      </c>
+      <c r="D40" t="s">
+        <v>148</v>
+      </c>
       <c r="E40" t="s">
         <v>58</v>
       </c>
@@ -1898,6 +1994,12 @@
       <c r="B41">
         <v>14</v>
       </c>
+      <c r="C41" t="s">
+        <v>90</v>
+      </c>
+      <c r="D41" t="s">
+        <v>167</v>
+      </c>
       <c r="E41" t="s">
         <v>59</v>
       </c>
@@ -1909,6 +2011,12 @@
       <c r="B42">
         <v>14</v>
       </c>
+      <c r="C42" t="s">
+        <v>166</v>
+      </c>
+      <c r="D42" t="s">
+        <v>106</v>
+      </c>
       <c r="E42" t="s">
         <v>60</v>
       </c>
@@ -1920,6 +2028,12 @@
       <c r="B43">
         <v>15</v>
       </c>
+      <c r="C43" t="s">
+        <v>169</v>
+      </c>
+      <c r="D43" t="s">
+        <v>90</v>
+      </c>
       <c r="E43" t="s">
         <v>62</v>
       </c>
@@ -1931,8 +2045,11 @@
       <c r="B44">
         <v>15</v>
       </c>
+      <c r="C44" t="s">
+        <v>90</v>
+      </c>
       <c r="E44" t="s">
-        <v>63</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1942,8 +2059,14 @@
       <c r="B45">
         <v>15</v>
       </c>
+      <c r="C45" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" t="s">
+        <v>92</v>
+      </c>
       <c r="E45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1953,8 +2076,14 @@
       <c r="B46">
         <v>16</v>
       </c>
+      <c r="C46" t="s">
+        <v>148</v>
+      </c>
+      <c r="D46" t="s">
+        <v>145</v>
+      </c>
       <c r="E46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1964,8 +2093,14 @@
       <c r="B47">
         <v>16</v>
       </c>
+      <c r="C47" t="s">
+        <v>171</v>
+      </c>
+      <c r="D47" t="s">
+        <v>91</v>
+      </c>
       <c r="E47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1975,8 +2110,14 @@
       <c r="B48">
         <v>16</v>
       </c>
+      <c r="C48" t="s">
+        <v>170</v>
+      </c>
+      <c r="D48" t="s">
+        <v>172</v>
+      </c>
       <c r="E48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1986,8 +2127,11 @@
       <c r="B49">
         <v>17</v>
       </c>
+      <c r="C49" t="s">
+        <v>174</v>
+      </c>
       <c r="E49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1997,8 +2141,11 @@
       <c r="B50">
         <v>17</v>
       </c>
+      <c r="C50" t="s">
+        <v>175</v>
+      </c>
       <c r="E50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2008,8 +2155,11 @@
       <c r="B51">
         <v>17</v>
       </c>
+      <c r="C51" t="s">
+        <v>173</v>
+      </c>
       <c r="E51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2019,8 +2169,11 @@
       <c r="B52">
         <v>17</v>
       </c>
+      <c r="C52" t="s">
+        <v>176</v>
+      </c>
       <c r="E52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2030,8 +2183,11 @@
       <c r="B53">
         <v>17</v>
       </c>
+      <c r="C53" t="s">
+        <v>177</v>
+      </c>
       <c r="E53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2041,8 +2197,14 @@
       <c r="B54">
         <v>18</v>
       </c>
+      <c r="C54" t="s">
+        <v>178</v>
+      </c>
+      <c r="D54" t="s">
+        <v>125</v>
+      </c>
       <c r="E54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2052,8 +2214,14 @@
       <c r="B55">
         <v>18</v>
       </c>
+      <c r="C55" t="s">
+        <v>179</v>
+      </c>
+      <c r="D55" t="s">
+        <v>96</v>
+      </c>
       <c r="E55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2063,8 +2231,14 @@
       <c r="B56">
         <v>18</v>
       </c>
+      <c r="C56" t="s">
+        <v>180</v>
+      </c>
+      <c r="D56" t="s">
+        <v>181</v>
+      </c>
       <c r="E56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2074,8 +2248,14 @@
       <c r="B57">
         <v>19</v>
       </c>
+      <c r="C57" t="s">
+        <v>183</v>
+      </c>
+      <c r="D57" t="s">
+        <v>90</v>
+      </c>
       <c r="E57" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2085,8 +2265,14 @@
       <c r="B58">
         <v>19</v>
       </c>
+      <c r="C58" t="s">
+        <v>182</v>
+      </c>
+      <c r="D58" t="s">
+        <v>184</v>
+      </c>
       <c r="E58" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2096,8 +2282,14 @@
       <c r="B59">
         <v>19</v>
       </c>
+      <c r="C59" t="s">
+        <v>162</v>
+      </c>
+      <c r="D59" t="s">
+        <v>122</v>
+      </c>
       <c r="E59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2107,8 +2299,14 @@
       <c r="B60">
         <v>20</v>
       </c>
+      <c r="C60" t="s">
+        <v>150</v>
+      </c>
+      <c r="D60" t="s">
+        <v>162</v>
+      </c>
       <c r="E60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2118,8 +2316,14 @@
       <c r="B61">
         <v>20</v>
       </c>
+      <c r="C61" t="s">
+        <v>186</v>
+      </c>
+      <c r="D61" t="s">
+        <v>103</v>
+      </c>
       <c r="E61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2129,8 +2333,14 @@
       <c r="B62">
         <v>20</v>
       </c>
+      <c r="C62" t="s">
+        <v>146</v>
+      </c>
+      <c r="D62" t="s">
+        <v>90</v>
+      </c>
       <c r="E62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2140,8 +2350,14 @@
       <c r="B63">
         <v>20</v>
       </c>
+      <c r="C63" t="s">
+        <v>185</v>
+      </c>
+      <c r="D63" t="s">
+        <v>91</v>
+      </c>
       <c r="E63" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2153,8 +2369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2166,112 +2382,112 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" t="s">
         <v>93</v>
-      </c>
-      <c r="C6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" t="s">
         <v>101</v>
-      </c>
-      <c r="D7" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" t="s">
         <v>109</v>
-      </c>
-      <c r="C12" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>